<commit_message>
Leer archivos de excel usando la funcion tabulate
</commit_message>
<xml_diff>
--- a/plantilla.xlsx
+++ b/plantilla.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\Scripts\python\tony\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\Scripts\python\tony\excel_files\excel_files_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="sueldos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -406,15 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -428,7 +429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -442,7 +443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -456,7 +457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -469,9 +470,9 @@
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>

</xml_diff>